<commit_message>
feat: use korean on excel
</commit_message>
<xml_diff>
--- a/examples/basic.xlsx
+++ b/examples/basic.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RATE</t>
+          <t>정률할인</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PRICE</t>
+          <t>정액할인</t>
         </is>
       </c>
       <c r="E3" t="n">

</xml_diff>

<commit_message>
example: add validation and description on excel example
</commit_message>
<xml_diff>
--- a/examples/basic.xlsx
+++ b/examples/basic.xlsx
@@ -137,6 +137,91 @@
 </styleSheet>
 </file>
 
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>시스템</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>쿠폰의 이름을 입력하세요.
+예시:
+- 신규회원 할인쿠폰
+- 주말 특별 할인
+- 1월 감사 쿠폰</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <t>쿠폰 타입을 선택하세요.
+▪ 즉시할인: 상품 페이지에서 자동으로 할인 적용
+▪ 다운로드쿠폰: 사용자가 다운로드 후 사용
+⚠ 주의: 드롭다운에서 선택하세요</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>쿠폰의 유효 기간을 일(day) 단위로 입력하세요.
+예시:
+- 7 → 7일간 유효
+- 30 → 30일간 유효
+⚠ 숫자만 입력 (1~365)</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <t>할인 방식을 선택하세요.
+▪ 정률할인: 정해진 비율(%)만큼 할인
+  - 다운로드쿠폰: 1~99%
+  - 즉시할인: 1~100%
+▪ 정액할인: 정해진 금액(원)만큼 할인
+  - 다운로드쿠폰: 10원 단위(10, 20, 30...)
+  - 즉시할인: 1원 이상
+▪ 수량별 정액할인: n개 구매 시 n번 할인
+  - 즉시할인 전용
+⚠ 주의: 드롭다운에서 선택하세요</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <t>할인 방식에 따른 할인 값을 입력하세요.
+▪ 정률할인: 1~100 사이의 숫자
+  - 10% 할인 → 10 입력 (% 기호 없이)
+  - 다운로드쿠폰은 최대 99까지
+▪ 정액할인: 할인 금액(원)
+  - 1000원 할인 → 1000 입력 (원 없이)
+  - 다운로드쿠폰은 10원 단위로
+▪ 수량별 정액할인: 1 이상의 숫자
+⚠ 주의: 숫자만 입력하세요</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <t>다운로드쿠폰의 일일 발급 개수를 입력하세요.
+예시:
+- 100 → 하루에 100개까지 발급
+- 빈칸 → 기본값(1개) 사용
+⚠ 즉시할인쿠폰은 비워두세요
+⚠ 숫자만 입력 (1 이상)</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>쿠폰을 적용할 상품 옵션 ID를 입력하세요.
+▪ 여러 개일 경우 쉼표(,)로 구분
+▪ 공백 없이 입력하세요
+예시:
+- 단일: 1234567890
+- 여러 개: 1234567890,9876543210,1122334455
+⚠ 필수 항목입니다
+⚠ 숫자와 쉼표만 입력</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -541,6 +626,28 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'즉시할인' 또는 '다운로드쿠폰'을 선택하세요" promptTitle="쿠폰타입" prompt="드롭다운에서 즉시할인 또는 다운로드쿠폰을 선택하세요" type="list">
+      <formula1>"즉시할인,다운로드쿠폰"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="1~365 사이의 숫자를 입력하세요" promptTitle="쿠폰유효기간" prompt="유효기간을 일(day) 단위로 입력하세요 (1~365)" type="whole" operator="between">
+      <formula1>1</formula1>
+      <formula2>365</formula2>
+    </dataValidation>
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'정률할인', '정액할인', '수량별 정액할인' 중 하나를 선택하세요" promptTitle="할인방식" prompt="드롭다운에서 할인 방식을 선택하세요" type="list">
+      <formula1>"정률할인,정액할인,수량별 정액할인"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="0" errorTitle="확인 필요" error="할인방식과 쿠폰타입에 따라 값의 범위가 다릅니다. 실행 시 재검증됩니다." promptTitle="할인금액/비율" prompt="정률할인: 1~100 (% 기호 없이)&#10;정액할인: 금액 (원 없이)&#10;수량별 정액할인: 1 이상" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1 이상의 숫자를 입력하세요. 즉시할인은 비워두세요." promptTitle="발급개수" prompt="다운로드쿠폰의 일일 발급 개수 (즉시할인은 비워두기)" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="옵션ID는 필수 입력입니다. 숫자를 쉼표로 구분하여 입력하세요." promptTitle="옵션ID" prompt="상품 옵션 ID를 입력하세요 (여러 개는 쉼표로 구분)" type="textLength" operator="greaterThan">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: remove datetime limit
</commit_message>
<xml_diff>
--- a/examples/basic.xlsx
+++ b/examples/basic.xlsx
@@ -166,7 +166,8 @@
 예시:
 - 7 → 7일간 유효
 - 30 → 30일간 유효
-⚠ 숫자만 입력 (1~365)</t>
+- 365 → 1년간 유효
+⚠ 숫자만 입력 (1~9999)</t>
       </text>
     </comment>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -630,9 +631,9 @@
     <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'즉시할인' 또는 '다운로드쿠폰'을 선택하세요" promptTitle="쿠폰타입" prompt="드롭다운에서 즉시할인 또는 다운로드쿠폰을 선택하세요" type="list">
       <formula1>"즉시할인,다운로드쿠폰"</formula1>
     </dataValidation>
-    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="1~365 사이의 숫자를 입력하세요" promptTitle="쿠폰유효기간" prompt="유효기간을 일(day) 단위로 입력하세요 (1~365)" type="whole" operator="between">
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="1~9999 사이의 숫자를 입력하세요" promptTitle="쿠폰유효기간" prompt="유효기간을 일(day) 단위로 입력하세요 (1~9999)" type="whole" operator="between">
       <formula1>1</formula1>
-      <formula2>365</formula2>
+      <formula2>9999</formula2>
     </dataValidation>
     <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'정률할인', '정액할인', '수량별 정액할인' 중 하나를 선택하세요" promptTitle="할인방식" prompt="드롭다운에서 할인 방식을 선택하세요" type="list">
       <formula1>"정률할인,정액할인,수량별 정액할인"</formula1>

</xml_diff>

<commit_message>
feat: add two columns on excel
</commit_message>
<xml_diff>
--- a/examples/basic.xlsx
+++ b/examples/basic.xlsx
@@ -512,7 +512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,8 +525,10 @@
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -557,10 +559,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>최소구매금액</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>최대할인금액</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>발급개수</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>옵션ID</t>
         </is>
@@ -589,7 +601,11 @@
         <v>10</v>
       </c>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>1234567890,1234567891</t>
         </is>
@@ -618,9 +634,15 @@
         <v>1000</v>
       </c>
       <c r="F3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H3" t="n">
         <v>100</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>9876543210</t>
         </is>

</xml_diff>

<commit_message>
fix: fix comments and descriptions of examples
</commit_message>
<xml_diff>
--- a/examples/basic.xlsx
+++ b/examples/basic.xlsx
@@ -156,8 +156,13 @@
       <text>
         <t>쿠폰 타입을 선택하세요.
 ▪ 즉시할인: 상품 페이지에서 자동으로 할인 적용
+  - 옵션ID 최대 10,000개
+  - 정률할인 1~100% 가능
 ▪ 다운로드쿠폰: 사용자가 다운로드 후 사용
-⚠ 주의: 드롭다운에서 선택하세요</t>
+  - 옵션ID 최대 100개
+  - 정률할인 1~99%만 가능
+  - 정액할인은 10원 단위
+⚠ 드롭다운에서 선택하세요</t>
       </text>
     </comment>
     <comment ref="C1" authorId="0" shapeId="0">
@@ -167,7 +172,7 @@
 - 7 → 7일간 유효
 - 30 → 30일간 유효
 - 365 → 1년간 유효
-⚠ 숫자만 입력 (1~9999)</t>
+⚠ 1 이상의 정수만 입력</t>
       </text>
     </comment>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -176,47 +181,78 @@
 ▪ 정률할인: 정해진 비율(%)만큼 할인
   - 다운로드쿠폰: 1~99%
   - 즉시할인: 1~100%
+  - 최대할인금액 필수 설정
 ▪ 정액할인: 정해진 금액(원)만큼 할인
-  - 다운로드쿠폰: 10원 단위(10, 20, 30...)
+  - 다운로드쿠폰: 최소 10원, 10원 단위
   - 즉시할인: 1원 이상
 ▪ 수량별 정액할인: n개 구매 시 n번 할인
-  - 즉시할인 전용
-⚠ 주의: 드롭다운에서 선택하세요</t>
+  - 즉시할인 전용 (다운로드쿠폰 불가)
+  - 1 이상의 정수
+⚠ 드롭다운에서 선택하세요</t>
       </text>
     </comment>
     <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <t>할인 방식에 따른 할인 값을 입력하세요.
-▪ 정률할인: 1~100 사이의 숫자
-  - 10% 할인 → 10 입력 (% 기호 없이)
-  - 다운로드쿠폰은 최대 99까지
-▪ 정액할인: 할인 금액(원)
-  - 1000원 할인 → 1000 입력 (원 없이)
-  - 다운로드쿠폰은 10원 단위로
-▪ 수량별 정액할인: 1 이상의 숫자
-⚠ 주의: 숫자만 입력하세요</t>
+▪ 정률할인:
+  - 다운로드쿠폰: 1~99 (10% → 10 입력)
+  - 즉시할인: 1~100 (100% 가능)
+▪ 정액할인:
+  - 다운로드쿠폰: 10원 단위 (1000 → 1000원)
+  - 즉시할인: 1원 이상 (1원 단위 가능)
+▪ 수량별 정액할인:
+  - 1 이상의 정수
+⚠ 숫자만 입력 (%, 원 기호 제외)</t>
       </text>
     </comment>
     <comment ref="F1" authorId="0" shapeId="0">
       <text>
+        <t>쿠폰 사용을 위한 최소 구매 금액을 입력하세요.
+▪ 다운로드쿠폰 전용:
+  - 예: 10000 → 1만원 이상 구매 시 사용 가능
+  - 빈칸 → 기본값 1원 (제한 없음)
+  - 1원 이상의 정수
+▪ 즉시할인쿠폰:
+  - 사용하지 않음 (비워두세요)
+⚠ 다운로드쿠폰만 입력, 즉시할인은 비워두기</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <t>정률할인 시 최대 할인 금액을 입력하세요.
+▪ 모든 쿠폰 필수 입력:
+  - 예: 5000 → 최대 5,000원까지만 할인
+  - 10% 할인이어도 5,000원 초과 불가
+  - 1원 이상의 정수
+▪ 정액할인의 경우:
+  - 할인금액과 동일하게 설정 권장
+  - 예: 3000원 할인 → 3000 입력
+⚠ 필수 항목 (비워두면 오류)</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
         <t>다운로드쿠폰의 일일 발급 개수를 입력하세요.
-예시:
-- 100 → 하루에 100개까지 발급
-- 빈칸 → 기본값(1개) 사용
-⚠ 즉시할인쿠폰은 비워두세요
-⚠ 숫자만 입력 (1 이상)</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+▪ 다운로드쿠폰:
+  - 예: 100 → 하루에 100개까지 발급
+  - 빈칸 → 기본값 1개
+  - 1 이상의 정수
+▪ 즉시할인쿠폰:
+  - 사용하지 않음 (비워두세요)
+⚠ 다운로드쿠폰만 입력, 즉시할인은 비워두기</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <t>쿠폰을 적용할 상품 옵션 ID를 입력하세요.
-▪ 여러 개일 경우 쉼표(,)로 구분
-▪ 공백 없이 입력하세요
-예시:
-- 단일: 1234567890
-- 여러 개: 1234567890,9876543210,1122334455
-⚠ 필수 항목입니다
-⚠ 숫자와 쉼표만 입력</t>
+▪ 입력 형식:
+  - 단일: 1234567890
+  - 여러 개: 1234567890,9876543210,1122334455
+  - 쉼표로 구분, 공백 없이
+▪ 개수 제한 (ADR 017):
+  - 즉시할인: 최대 10,000개
+  - 다운로드쿠폰: 최대 100개
+⚠ 필수 항목 (양의 정수만)</t>
       </text>
     </comment>
   </commentList>
@@ -649,24 +685,29 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="8">
     <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'즉시할인' 또는 '다운로드쿠폰'을 선택하세요" promptTitle="쿠폰타입" prompt="드롭다운에서 즉시할인 또는 다운로드쿠폰을 선택하세요" type="list">
       <formula1>"즉시할인,다운로드쿠폰"</formula1>
     </dataValidation>
-    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="1~9999 사이의 숫자를 입력하세요" promptTitle="쿠폰유효기간" prompt="유효기간을 일(day) 단위로 입력하세요 (1~9999)" type="whole" operator="between">
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="1 이상의 정수를 입력하세요" promptTitle="쿠폰유효기간" prompt="유효기간을 일(day) 단위로 입력하세요 (1 이상)" type="whole" operator="greaterThanOrEqual">
       <formula1>1</formula1>
-      <formula2>9999</formula2>
     </dataValidation>
     <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'정률할인', '정액할인', '수량별 정액할인' 중 하나를 선택하세요" promptTitle="할인방식" prompt="드롭다운에서 할인 방식을 선택하세요" type="list">
       <formula1>"정률할인,정액할인,수량별 정액할인"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="0" errorTitle="확인 필요" error="할인방식과 쿠폰타입에 따라 값의 범위가 다릅니다. 실행 시 재검증됩니다." promptTitle="할인금액/비율" prompt="정률할인: 1~100 (% 기호 없이)&#10;정액할인: 금액 (원 없이)&#10;수량별 정액할인: 1 이상" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="0" errorTitle="확인 필요" error="쿠폰타입과 할인방식에 따라 값의 범위가 다릅니다.&#10;- 다운로드쿠폰 정률할인: 1~99&#10;- 즉시할인 정률할인: 1~100&#10;- 다운로드쿠폰 정액할인: 10원 단위&#10;- 즉시할인 정액할인: 1원 이상" promptTitle="할인금액/비율" prompt="정률할인: 1~100 (% 기호 없이)&#10;정액할인: 금액 (원 없이)&#10;수량별 정액할인: 1 이상" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1 이상의 숫자를 입력하세요. 즉시할인은 비워두세요." promptTitle="발급개수" prompt="다운로드쿠폰의 일일 발급 개수 (즉시할인은 비워두기)" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1원 이상의 정수를 입력하세요. 즉시할인은 비워두세요." promptTitle="최소구매금액" prompt="다운로드쿠폰 전용 (즉시할인은 비워두기)&#10;예: 10000 → 1만원 이상 구매 시 사용 가능&#10;빈칸 → 기본값 1원 (제한 없음)" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="옵션ID는 필수 입력입니다. 숫자를 쉼표로 구분하여 입력하세요." promptTitle="옵션ID" prompt="상품 옵션 ID를 입력하세요 (여러 개는 쉼표로 구분)" type="textLength" operator="greaterThan">
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="최대할인금액은 필수입니다. 1원 이상의 정수를 입력하세요." promptTitle="최대할인금액" prompt="정률할인 시 최대 할인 금액 (필수)&#10;예: 5000 → 최대 5,000원까지만 할인&#10;정액할인은 할인금액과 동일하게 설정 권장" type="whole" operator="greaterThanOrEqual">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1 이상의 숫자를 입력하세요. 즉시할인은 비워두세요." promptTitle="발급개수" prompt="다운로드쿠폰의 일일 발급 개수 (즉시할인은 비워두기)&#10;예: 100 → 하루에 100개까지 발급&#10;빈칸 → 기본값 1개" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="옵션ID는 필수 입력입니다. 숫자를 쉼표로 구분하여 입력하세요." promptTitle="옵션ID" prompt="상품 옵션 ID를 입력하세요 (여러 개는 쉼표로 구분)&#10;즉시할인: 최대 10,000개&#10;다운로드쿠폰: 최대 100개" type="textLength" operator="greaterThan">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat: make coupon type column's instant coupon type name full name
</commit_message>
<xml_diff>
--- a/examples/basic.xlsx
+++ b/examples/basic.xlsx
@@ -155,7 +155,7 @@
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <t>쿠폰 타입을 선택하세요.
-▪ 즉시할인: 상품 페이지에서 자동으로 할인 적용
+▪ 즉시할인쿠폰: 상품 페이지에서 자동으로 할인 적용
   - 옵션ID 최대 10,000개
   - 정률할인 1~100% 가능
 ▪ 다운로드쿠폰: 사용자가 다운로드 후 사용
@@ -180,13 +180,13 @@
         <t>할인 방식을 선택하세요.
 ▪ 정률할인: 정해진 비율(%)만큼 할인
   - 다운로드쿠폰: 1~99%
-  - 즉시할인: 1~100%
+  - 즉시할인쿠폰: 1~100%
   - 최대할인금액 필수 설정
 ▪ 정액할인: 정해진 금액(원)만큼 할인
   - 다운로드쿠폰: 최소 10원, 10원 단위
-  - 즉시할인: 1원 이상
+  - 즉시할인쿠폰: 1원 이상
 ▪ 수량별 정액할인: n개 구매 시 n번 할인
-  - 즉시할인 전용 (다운로드쿠폰 불가)
+  - 즉시할인쿠폰 전용 (다운로드쿠폰 불가)
   - 1 이상의 정수
 ⚠ 드롭다운에서 선택하세요</t>
       </text>
@@ -196,10 +196,10 @@
         <t>할인 방식에 따른 할인 값을 입력하세요.
 ▪ 정률할인:
   - 다운로드쿠폰: 1~99 (10% → 10 입력)
-  - 즉시할인: 1~100 (100% 가능)
+  - 즉시할인쿠폰: 1~100 (100% 가능)
 ▪ 정액할인:
   - 다운로드쿠폰: 10원 단위 (1000 → 1000원)
-  - 즉시할인: 1원 이상 (1원 단위 가능)
+  - 즉시할인쿠폰: 1원 이상 (1원 단위 가능)
 ▪ 수량별 정액할인:
   - 1 이상의 정수
 ⚠ 숫자만 입력 (%, 원 기호 제외)</t>
@@ -214,7 +214,7 @@
   - 1원 이상의 정수
 ▪ 즉시할인쿠폰:
   - 사용하지 않음 (비워두세요)
-⚠ 다운로드쿠폰만 입력, 즉시할인은 비워두기</t>
+⚠ 다운로드쿠폰만 입력, 즉시할인쿠폰은 비워두기</t>
       </text>
     </comment>
     <comment ref="G1" authorId="0" shapeId="0">
@@ -239,7 +239,7 @@
   - 1 이상의 정수
 ▪ 즉시할인쿠폰:
   - 사용하지 않음 (비워두세요)
-⚠ 다운로드쿠폰만 입력, 즉시할인은 비워두기</t>
+⚠ 다운로드쿠폰만 입력, 즉시할인쿠폰은 비워두기</t>
       </text>
     </comment>
     <comment ref="I1" authorId="0" shapeId="0">
@@ -248,9 +248,9 @@
 ▪ 입력 형식:
   - 단일: 1234567890
   - 여러 개: 1234567890,9876543210,1122334455
-  - 쉼표로 구분, 공백 없이
+  - 쉬표로 구분, 공백 없이
 ▪ 개수 제한 (ADR 017):
-  - 즉시할인: 최대 10,000개
+  - 즉시할인쿠폰: 최대 10,000개
   - 다운로드쿠폰: 최대 100개
 ⚠ 필수 항목 (양의 정수만)</t>
       </text>
@@ -622,7 +622,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>즉시할인</t>
+          <t>즉시할인쿠폰</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -686,8 +686,8 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'즉시할인' 또는 '다운로드쿠폰'을 선택하세요" promptTitle="쿠폰타입" prompt="드롭다운에서 즉시할인 또는 다운로드쿠폰을 선택하세요" type="list">
-      <formula1>"즉시할인,다운로드쿠폰"</formula1>
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'즉시할인쿠폰' 또는 '다운로드쿠폰'을 선택하세요" promptTitle="쿠폰타입" prompt="드롭다운에서 즉시할인쿠폰 또는 다운로드쿠폰을 선택하세요" type="list">
+      <formula1>"즉시할인쿠폰,다운로드쿠폰"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="1 이상의 정수를 입력하세요" promptTitle="쿠폰유효기간" prompt="유효기간을 일(day) 단위로 입력하세요 (1 이상)" type="whole" operator="greaterThanOrEqual">
       <formula1>1</formula1>
@@ -695,16 +695,16 @@
     <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="'정률할인', '정액할인', '수량별 정액할인' 중 하나를 선택하세요" promptTitle="할인방식" prompt="드롭다운에서 할인 방식을 선택하세요" type="list">
       <formula1>"정률할인,정액할인,수량별 정액할인"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="0" errorTitle="확인 필요" error="쿠폰타입과 할인방식에 따라 값의 범위가 다릅니다.&#10;- 다운로드쿠폰 정률할인: 1~99&#10;- 즉시할인 정률할인: 1~100&#10;- 다운로드쿠폰 정액할인: 10원 단위&#10;- 즉시할인 정액할인: 1원 이상" promptTitle="할인금액/비율" prompt="정률할인: 1~100 (% 기호 없이)&#10;정액할인: 금액 (원 없이)&#10;수량별 정액할인: 1 이상" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="0" errorTitle="확인 필요" error="쿠폰타입과 할인방식에 따라 값의 범위가 다릅니다.&#10;- 다운로드쿠폰 정률할인: 1~99&#10;- 즉시할인쿠폰 정률할인: 1~100&#10;- 다운로드쿠폰 정액할인: 10원 단위&#10;- 즉시할인쿠폰 정액할인: 1원 이상" promptTitle="할인금액/비율" prompt="정률할인: 1~100 (% 기호 없이)&#10;정액할인: 금액 (원 없이)&#10;수량별 정액할인: 1 이상" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1원 이상의 정수를 입력하세요. 즉시할인은 비워두세요." promptTitle="최소구매금액" prompt="다운로드쿠폰 전용 (즉시할인은 비워두기)&#10;예: 10000 → 1만원 이상 구매 시 사용 가능&#10;빈칸 → 기본값 1원 (제한 없음)" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1원 이상의 정수를 입력하세요. 즉시할인쿠폰은 비워두세요." promptTitle="최소구매금액" prompt="다운로드쿠폰 전용 (즉시할인쿠폰은 비워두기)&#10;예: 10000 → 1만원 이상 구매 시 사용 가능&#10;빈칸 → 기본값 1원 (제한 없음)" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="최대할인금액은 필수입니다. 1원 이상의 정수를 입력하세요." promptTitle="최대할인금액" prompt="정률할인 시 최대 할인 금액 (필수)&#10;예: 5000 → 최대 5,000원까지만 할인&#10;정액할인은 할인금액과 동일하게 설정 권장" type="whole" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1 이상의 숫자를 입력하세요. 즉시할인은 비워두세요." promptTitle="발급개수" prompt="다운로드쿠폰의 일일 발급 개수 (즉시할인은 비워두기)&#10;예: 100 → 하루에 100개까지 발급&#10;빈칸 → 기본값 1개" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
+    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" errorTitle="확인 필요" error="다운로드쿠폰인 경우 1 이상의 숫자를 입력하세요. 즉시할인쿠폰은 비워두세요." promptTitle="발급개수" prompt="다운로드쿠폰의 일일 발급 개수 (즉시할인쿠폰은 비워두기)&#10;예: 100 → 하루에 100개까지 발급&#10;빈칸 → 기본값 1개" type="whole" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" errorTitle="입력 오류" error="옵션ID는 필수 입력입니다. 숫자를 쉼표로 구분하여 입력하세요." promptTitle="옵션ID" prompt="상품 옵션 ID를 입력하세요 (여러 개는 쉼표로 구분)&#10;즉시할인: 최대 10,000개&#10;다운로드쿠폰: 최대 100개" type="textLength" operator="greaterThan">

</xml_diff>